<commit_message>
Updated figures and source data
</commit_message>
<xml_diff>
--- a/plots.xlsx
+++ b/plots.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/solexa_rouskin/projects/mfallan/SARS2_genome_structure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B111585A-E645-E040-82BF-DF03E5CC9106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91455295-4B2E-D943-8077-171CDFAE67F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10920" yWindow="500" windowWidth="24920" windowHeight="21900" activeTab="1" xr2:uid="{75BAA94C-F7BE-AB4A-A3FF-AD69AFCE8A9B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="135">
   <si>
     <t>Projects</t>
   </si>
@@ -173,153 +173,12 @@
     <t>VeroE6_FSE_k2_c2, Huh7_FSE_k2_c1</t>
   </si>
   <si>
-    <t>Huh7_1_bvAll</t>
-  </si>
-  <si>
-    <t>EM_Clustering_200b_ge2muts</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvge2</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_vs_Huh7_FSE_scatter.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_vs_Huh7_FSE_diffbar.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_vs_Huh7_FSE_bar.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_vs_Huh7_FSE_k2_scatmat.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_c1_vs_Huh7_FSE_c2_bar.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_c2_vs_Huh7_FSE_c1_bar.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_c1_vs_Huh7_FSE_c2_diffbar.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_c2_vs_Huh7_FSE_c1_diffbar.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_1_all_vs_ge2.pdf</t>
-  </si>
-  <si>
     <t>Huh7_FSE</t>
   </si>
   <si>
-    <t>Huh7_1_bvAll, Huh7_1_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_2_bvAll</t>
-  </si>
-  <si>
-    <t>Huh7_2_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_3_bvAll</t>
-  </si>
-  <si>
-    <t>Huh7_3_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_4_bvAll</t>
-  </si>
-  <si>
-    <t>Huh7_4_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_5_bvAll</t>
-  </si>
-  <si>
-    <t>Huh7_5_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_6_bvAll</t>
-  </si>
-  <si>
-    <t>Huh7_6_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_7_bvAll</t>
-  </si>
-  <si>
-    <t>Huh7_7_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_2_bvAll, Huh7_2_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_3_bvAll, Huh7_3_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_4_bvAll, Huh7_4_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_5_bvAll, Huh7_5_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_6_bvAll, Huh7_6_bvge2</t>
-  </si>
-  <si>
-    <t>Huh7_7_bvAll, Huh7_7_bvge2</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_3_all_vs_ge2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_2_all_vs_ge2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_4_all_vs_ge2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_5_all_vs_ge2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_6_all_vs_ge2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_7_all_vs_ge2.pdf</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvAll_c2</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvAll_c1</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvge2_c1</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvge2_c2</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvAll_c1, Huh7_1_bvAll_c2</t>
-  </si>
-  <si>
-    <t>Huh7_1_bvge2_c1, Huh7_1_bvge2_c2</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_1_all.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Huh7_1_ge2.pdf</t>
-  </si>
-  <si>
     <t>{"mplrc": {"font.size": 10}, "label_titles": true, "sharex": true}</t>
   </si>
   <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_c2_vs_Huh7_FSE_c1_scatter.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/VeroE6_FSE_c1_vs_Huh7_FSE_c2_scatter.pdf</t>
-  </si>
-  <si>
     <t>{"mplrc": {"font.size": 10}}</t>
   </si>
   <si>
@@ -368,9 +227,6 @@
     <t>FSE_30kb</t>
   </si>
   <si>
-    <t>SARS2_smallF_vitro_2p5DMS</t>
-  </si>
-  <si>
     <t>SARS2_virion_Frameshift</t>
   </si>
   <si>
@@ -407,24 +263,6 @@
     <t>VeroE6_FSE_rep2, VeroE6_FSE</t>
   </si>
   <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4_92.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4_283.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4_3kb.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4_30kb.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4_Vero2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4_Huh7.pdf</t>
-  </si>
-  <si>
     <t>Huh7_FSE_sig005</t>
   </si>
   <si>
@@ -530,15 +368,6 @@
     <t>sars2_smallframe</t>
   </si>
   <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4a_short1.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4a_short2.pdf</t>
-  </si>
-  <si>
-    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_resubmission_210630/scripts/Fig4a_short3.pdf</t>
-  </si>
-  <si>
     <t>FSE_small11, FSE_small12</t>
   </si>
   <si>
@@ -546,6 +375,69 @@
   </si>
   <si>
     <t>FSE_small12, FSE_small22</t>
+  </si>
+  <si>
+    <t>SARS2smallframe</t>
+  </si>
+  <si>
+    <t>{"mplrc": {"font.size": 10}, "ymax": 0.2, "xmax": 0.2, "matched_indexes": false}</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4_92.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4_283.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4_3kb.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4_30kb.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4_Vero2.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4_Huh7.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_vs_Huh7_FSE_scatter.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_vs_Huh7_FSE_diffbar.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_vs_Huh7_FSE_bar.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_vs_Huh7_FSE_k2_scatmat.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_c1_vs_Huh7_FSE_c2_bar.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_c2_vs_Huh7_FSE_c1_bar.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_c1_vs_Huh7_FSE_c2_scatter.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_c2_vs_Huh7_FSE_c1_scatter.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_c1_vs_Huh7_FSE_c2_diffbar.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/VeroE6_FSE_c2_vs_Huh7_FSE_c1_diffbar.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4a_short1.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4a_short2.pdf</t>
+  </si>
+  <si>
+    <t>/lab/solexa_rouskin/projects/mfallan/SARS2_genome_structure/scripts/Fig4a_short3.pdf</t>
   </si>
 </sst>
 </file>
@@ -943,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D45D2CB-82A4-C34F-A2A3-03CA5D07FEF8}">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,7 +952,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1072,7 +964,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
@@ -1092,7 +984,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1101,7 +993,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -1121,7 +1013,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1197,7 +1089,7 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -1308,7 +1200,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -1343,7 +1235,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -1369,7 +1261,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -1378,7 +1270,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -1387,7 +1279,7 @@
         <v>30</v>
       </c>
       <c r="G12">
-        <v>829</v>
+        <v>13434</v>
       </c>
       <c r="M12">
         <v>2</v>
@@ -1395,8 +1287,8 @@
       <c r="N12" t="s">
         <v>24</v>
       </c>
-      <c r="O12" t="s">
-        <v>25</v>
+      <c r="O12">
+        <v>1</v>
       </c>
       <c r="P12" t="b">
         <v>0</v>
@@ -1404,7 +1296,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1413,7 +1305,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -1422,7 +1314,7 @@
         <v>30</v>
       </c>
       <c r="G13">
-        <v>829</v>
+        <v>13434</v>
       </c>
       <c r="M13">
         <v>2</v>
@@ -1430,8 +1322,8 @@
       <c r="N13" t="s">
         <v>24</v>
       </c>
-      <c r="O13" t="s">
-        <v>25</v>
+      <c r="O13">
+        <v>2</v>
       </c>
       <c r="P13" t="b">
         <v>0</v>
@@ -1448,25 +1340,25 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="G14">
-        <v>5836</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N14" t="s">
         <v>24</v>
       </c>
-      <c r="O14" t="s">
-        <v>25</v>
+      <c r="O14">
+        <v>1</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -1483,25 +1375,19 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
         <v>30</v>
       </c>
       <c r="G15">
-        <v>5836</v>
+        <v>13367</v>
       </c>
       <c r="M15">
-        <v>2</v>
-      </c>
-      <c r="N15" t="s">
-        <v>24</v>
-      </c>
-      <c r="O15" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P15" t="b">
         <v>0</v>
@@ -1515,34 +1401,28 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="G16">
-        <v>7033</v>
+        <v>13369</v>
       </c>
       <c r="M16">
-        <v>2</v>
-      </c>
-      <c r="N16" t="s">
-        <v>24</v>
-      </c>
-      <c r="O16" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1553,331 +1433,267 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
         <v>30</v>
       </c>
       <c r="G17">
-        <v>7033</v>
+        <v>13367</v>
       </c>
       <c r="M17">
-        <v>2</v>
-      </c>
-      <c r="N17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O17" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
         <v>30</v>
       </c>
       <c r="G18">
-        <v>9870</v>
+        <v>13369</v>
       </c>
       <c r="M18">
-        <v>2</v>
-      </c>
-      <c r="N18" t="s">
-        <v>24</v>
-      </c>
-      <c r="O18" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19">
-        <v>9870</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="M19">
-        <v>2</v>
-      </c>
-      <c r="N19" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20">
-        <v>11830</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F20" s="4"/>
       <c r="M20">
-        <v>2</v>
-      </c>
-      <c r="N20" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21">
-        <v>11830</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="F21" s="4"/>
       <c r="M21">
-        <v>2</v>
-      </c>
-      <c r="N21" t="s">
-        <v>24</v>
-      </c>
-      <c r="O21" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22">
-        <v>15239</v>
-      </c>
-      <c r="M22">
-        <v>2</v>
-      </c>
-      <c r="N22" t="s">
-        <v>24</v>
-      </c>
-      <c r="O22" t="s">
-        <v>25</v>
-      </c>
-      <c r="P22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" t="s">
-        <v>47</v>
+        <v>98</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G23">
-        <v>15239</v>
+        <v>19</v>
+      </c>
+      <c r="H23">
+        <v>157</v>
       </c>
       <c r="M23">
-        <v>2</v>
-      </c>
-      <c r="N23" t="s">
-        <v>24</v>
-      </c>
-      <c r="O23" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
+        <v>98</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G24">
-        <v>28648</v>
+        <v>19</v>
+      </c>
+      <c r="H24">
+        <v>157</v>
       </c>
       <c r="M24">
-        <v>2</v>
-      </c>
-      <c r="N24" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25">
-        <v>28648</v>
+        <v>107</v>
       </c>
       <c r="M25">
-        <v>2</v>
-      </c>
-      <c r="N25" t="s">
-        <v>24</v>
-      </c>
-      <c r="O25" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="P25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26">
-        <v>829</v>
+        <v>107</v>
       </c>
       <c r="M26">
         <v>2</v>
@@ -1892,593 +1708,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27">
-        <v>829</v>
-      </c>
-      <c r="M27">
-        <v>2</v>
-      </c>
-      <c r="N27" t="s">
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2">
+        <v>2</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O27">
-        <v>2</v>
-      </c>
-      <c r="P27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28">
-        <v>829</v>
-      </c>
-      <c r="M28">
-        <v>2</v>
-      </c>
-      <c r="N28" t="s">
-        <v>24</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29">
-        <v>829</v>
-      </c>
-      <c r="M29">
-        <v>2</v>
-      </c>
-      <c r="N29" t="s">
-        <v>24</v>
-      </c>
-      <c r="O29">
-        <v>2</v>
-      </c>
-      <c r="P29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30">
-        <v>13434</v>
-      </c>
-      <c r="M30">
-        <v>2</v>
-      </c>
-      <c r="N30" t="s">
-        <v>24</v>
-      </c>
-      <c r="O30">
-        <v>1</v>
-      </c>
-      <c r="P30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31">
-        <v>13434</v>
-      </c>
-      <c r="M31">
-        <v>2</v>
-      </c>
-      <c r="N31" t="s">
-        <v>24</v>
-      </c>
-      <c r="O31">
-        <v>2</v>
-      </c>
-      <c r="P31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" t="s">
-        <v>30</v>
-      </c>
-      <c r="G32">
-        <v>13459</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="P32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>108</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" t="s">
-        <v>30</v>
-      </c>
-      <c r="G33">
-        <v>13367</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="P33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
-        <v>114</v>
-      </c>
-      <c r="F34" t="s">
-        <v>116</v>
-      </c>
-      <c r="G34">
-        <v>13369</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="P34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>112</v>
-      </c>
-      <c r="F35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35">
-        <v>13367</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="P35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36">
-        <v>13369</v>
-      </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="P36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>136</v>
-      </c>
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>137</v>
-      </c>
-      <c r="D37" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="M37">
-        <v>1</v>
-      </c>
-      <c r="P37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>142</v>
-      </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>137</v>
-      </c>
-      <c r="D38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>139</v>
-      </c>
-      <c r="F38" s="4"/>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="P38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>140</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>137</v>
-      </c>
-      <c r="D39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="P39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2">
-        <v>1</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>153</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41" t="s">
-        <v>154</v>
-      </c>
-      <c r="G41">
-        <v>19</v>
-      </c>
-      <c r="H41">
-        <v>157</v>
-      </c>
-      <c r="M41">
-        <v>1</v>
-      </c>
-      <c r="P41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>155</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>152</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" t="s">
-        <v>155</v>
-      </c>
-      <c r="F42" t="s">
-        <v>154</v>
-      </c>
-      <c r="G42">
-        <v>19</v>
-      </c>
-      <c r="H42">
-        <v>157</v>
-      </c>
-      <c r="M42">
-        <v>1</v>
-      </c>
-      <c r="P42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>159</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>160</v>
-      </c>
-      <c r="F43" t="s">
-        <v>161</v>
-      </c>
-      <c r="M43">
-        <v>1</v>
-      </c>
-      <c r="P43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>162</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
-        <v>160</v>
-      </c>
-      <c r="F44" t="s">
-        <v>161</v>
-      </c>
-      <c r="M44">
-        <v>2</v>
-      </c>
-      <c r="N44" t="s">
-        <v>24</v>
-      </c>
-      <c r="O44">
-        <v>1</v>
-      </c>
-      <c r="P44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2">
-        <v>2</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O45" s="2">
-        <v>2</v>
-      </c>
-      <c r="P45" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
+      <c r="O27" s="2">
+        <v>2</v>
+      </c>
+      <c r="P27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2488,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E61DE97-E1CB-6140-887E-D306D7338148}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A18" sqref="A18:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2521,13 +1789,13 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2535,13 +1803,13 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2549,13 +1817,13 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2563,13 +1831,13 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2577,13 +1845,13 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2591,13 +1859,13 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2608,7 +1876,7 @@
         <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -2622,7 +1890,7 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -2636,10 +1904,10 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2650,7 +1918,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -2664,10 +1932,10 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2678,10 +1946,10 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2692,10 +1960,10 @@
         <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2706,10 +1974,10 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2720,7 +1988,7 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -2734,7 +2002,7 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
         <v>32</v>
@@ -2742,114 +2010,114 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>79</v>
+        <v>53</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2857,13 +2125,13 @@
         <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2871,153 +2139,27 @@
         <v>34</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>102</v>
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" t="s">
-        <v>150</v>
-      </c>
-      <c r="D33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C35" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C36" t="s">
-        <v>166</v>
-      </c>
-      <c r="D36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" t="s">
-        <v>167</v>
-      </c>
-      <c r="D37" t="s">
-        <v>135</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>